<commit_message>
them import qua trinh dong bao hiem trong chuc nang import thông tin nhan vien
</commit_message>
<xml_diff>
--- a/server/upload/human-resource/templateImport/templateImportEmployee.xlsx
+++ b/server/upload/human-resource/templateImport/templateImportEmployee.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hung Cuong\Desktop\DATN\Mẫu file Import\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C8F0AA-A5E5-4595-809B-7F0F1065AE21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.Nhân viên" sheetId="2" r:id="rId1"/>
@@ -12,28 +18,21 @@
     <sheet name="3.HS Nhân viên - Bằng cấp" sheetId="10" r:id="rId3"/>
     <sheet name="4.HS Nhân viên - Chứng chỉ" sheetId="11" r:id="rId4"/>
     <sheet name="5.HS Nhân viên - Hợp đồng" sheetId="12" r:id="rId5"/>
-    <sheet name="6.HS Nhân viên - Tài liệu" sheetId="13" r:id="rId6"/>
-    <sheet name="Cấu hình - Drop down list" sheetId="14" r:id="rId7"/>
+    <sheet name="7.HS Nhân viên - Bảo hiểm XH" sheetId="15" r:id="rId6"/>
+    <sheet name="8.HS Nhân viên - Tài liệu" sheetId="13" r:id="rId7"/>
+    <sheet name="Cấu hình - Drop down list" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="154">
   <si>
     <t>STT</t>
   </si>
@@ -500,7 +499,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
   </numFmts>
@@ -750,7 +749,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -787,7 +786,7 @@
         <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BCEF7FA2-8B72-4032-A6F2-CB61215F787B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCEF7FA2-8B72-4032-A6F2-CB61215F787B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -796,7 +795,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="9576" y="95250"/>
-          <a:ext cx="6165799" cy="1010770"/>
+          <a:ext cx="5905449" cy="1010770"/>
           <a:chOff x="3988207" y="294670"/>
           <a:chExt cx="5925062" cy="1019954"/>
         </a:xfrm>
@@ -807,7 +806,7 @@
           <xdr:cNvPr id="3" name="TextBox 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{306F6257-7476-4364-90D0-6CB9E71A292F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{306F6257-7476-4364-90D0-6CB9E71A292F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -956,7 +955,7 @@
           <xdr:cNvPr id="4" name="Picture 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79D01B0B-92F9-4CDA-9880-C480E8CCAD54}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79D01B0B-92F9-4CDA-9880-C480E8CCAD54}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1011,7 +1010,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60D929C9-291C-4E57-BAC9-B18D37E4DCB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60D929C9-291C-4E57-BAC9-B18D37E4DCB5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1084,7 +1083,7 @@
         <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BF77145-52E9-41C7-BBF6-36887C921260}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF77145-52E9-41C7-BBF6-36887C921260}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1093,7 +1092,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="9576" y="95250"/>
-          <a:ext cx="6146749" cy="1010770"/>
+          <a:ext cx="5905449" cy="1010770"/>
           <a:chOff x="3988207" y="294670"/>
           <a:chExt cx="5925062" cy="1019954"/>
         </a:xfrm>
@@ -1104,7 +1103,7 @@
           <xdr:cNvPr id="3" name="TextBox 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D35B0DEE-0287-4734-91FF-420814048D5D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D35B0DEE-0287-4734-91FF-420814048D5D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1253,7 +1252,7 @@
           <xdr:cNvPr id="4" name="Picture 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3A79ECEE-7E58-44BC-A54B-AE6D39E91DBC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A79ECEE-7E58-44BC-A54B-AE6D39E91DBC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1308,7 +1307,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BABF3CBD-639F-4712-9A07-E35EF95B210F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BABF3CBD-639F-4712-9A07-E35EF95B210F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1381,7 +1380,7 @@
         <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A8E3B9FC-1A5F-4495-877D-74354C56C0A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8E3B9FC-1A5F-4495-877D-74354C56C0A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1390,7 +1389,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="9576" y="95250"/>
-          <a:ext cx="6159449" cy="1010770"/>
+          <a:ext cx="5905449" cy="1010770"/>
           <a:chOff x="3988207" y="294670"/>
           <a:chExt cx="5925062" cy="1019954"/>
         </a:xfrm>
@@ -1401,7 +1400,7 @@
           <xdr:cNvPr id="3" name="TextBox 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{714AD7B5-FE72-4CBD-861E-4F604C3D01F2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{714AD7B5-FE72-4CBD-861E-4F604C3D01F2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1550,7 +1549,7 @@
           <xdr:cNvPr id="4" name="Picture 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E8D3A97B-A202-4ECA-8D19-0EFBD52F83DC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D3A97B-A202-4ECA-8D19-0EFBD52F83DC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1605,7 +1604,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C2289521-A382-4D62-B295-BBF31F60AB32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2289521-A382-4D62-B295-BBF31F60AB32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1678,7 +1677,7 @@
         <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D8C2ABAF-2B07-457C-8EB9-67F783AD20A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8C2ABAF-2B07-457C-8EB9-67F783AD20A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1687,7 +1686,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="9576" y="95250"/>
-          <a:ext cx="6146749" cy="1010770"/>
+          <a:ext cx="5905449" cy="1010770"/>
           <a:chOff x="3988207" y="294670"/>
           <a:chExt cx="5925062" cy="1019954"/>
         </a:xfrm>
@@ -1698,7 +1697,7 @@
           <xdr:cNvPr id="3" name="TextBox 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D900596-806A-47EF-9B17-46D89BE18F20}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D900596-806A-47EF-9B17-46D89BE18F20}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1847,7 +1846,7 @@
           <xdr:cNvPr id="4" name="Picture 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0B427B58-0998-4700-9F24-A61763995968}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B427B58-0998-4700-9F24-A61763995968}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1902,7 +1901,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC70B2E9-30CF-491F-A509-1EEA013765CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC70B2E9-30CF-491F-A509-1EEA013765CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1975,7 +1974,7 @@
         <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AC2CC646-2D82-42A8-A078-7D088E8692BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC2CC646-2D82-42A8-A078-7D088E8692BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1984,7 +1983,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="9576" y="95250"/>
-          <a:ext cx="6172149" cy="1010770"/>
+          <a:ext cx="5905449" cy="1010770"/>
           <a:chOff x="3988207" y="294670"/>
           <a:chExt cx="5925062" cy="1019954"/>
         </a:xfrm>
@@ -1995,7 +1994,7 @@
           <xdr:cNvPr id="3" name="TextBox 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92D67AE6-DEFB-4E02-9346-5D0FCCF37631}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92D67AE6-DEFB-4E02-9346-5D0FCCF37631}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2144,7 +2143,7 @@
           <xdr:cNvPr id="4" name="Picture 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B00E36F9-8556-4D73-8BA8-A5469B9390C7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B00E36F9-8556-4D73-8BA8-A5469B9390C7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2199,7 +2198,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6948AADD-C768-43CC-BAA6-6FD56FC7EC2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6948AADD-C768-43CC-BAA6-6FD56FC7EC2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2262,8 +2261,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>153520</xdr:rowOff>
     </xdr:to>
@@ -2272,7 +2271,7 @@
         <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1742CE6D-B6EC-4C27-82A5-67D7DD11C6B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A745D885-7DFE-4BEE-A00D-8C05656A9A75}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2281,7 +2280,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="9576" y="95250"/>
-          <a:ext cx="6124524" cy="1010770"/>
+          <a:ext cx="5905449" cy="1010770"/>
           <a:chOff x="3988207" y="294670"/>
           <a:chExt cx="5925062" cy="1019954"/>
         </a:xfrm>
@@ -2292,7 +2291,7 @@
           <xdr:cNvPr id="3" name="TextBox 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{06740C46-960B-4839-A6A5-C556CB3D83A6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04AE153B-2DA0-4FCF-9D29-1DC52E30DC81}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2441,7 +2440,304 @@
           <xdr:cNvPr id="4" name="Picture 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{676B4BF4-916F-4710-A652-86DF7BC53E22}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{996BE68E-14BD-497D-99EF-B1B40138815F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3988207" y="294670"/>
+            <a:ext cx="709979" cy="904876"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:grpFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>72839</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79659FCE-6380-4B15-9E71-9DE7344F6D34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1647825" y="723900"/>
+          <a:ext cx="6858000" cy="301439"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>MẪU IMPORT BẢO HIỂM XÃ HỘI</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9576</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>153520</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1742CE6D-B6EC-4C27-82A5-67D7DD11C6B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9576" y="95250"/>
+          <a:ext cx="5905449" cy="1010770"/>
+          <a:chOff x="3988207" y="294670"/>
+          <a:chExt cx="5925062" cy="1019954"/>
+        </a:xfrm>
+        <a:noFill/>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="TextBox 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06740C46-960B-4839-A6A5-C556CB3D83A6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4915148" y="381173"/>
+            <a:ext cx="4998121" cy="933451"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:grpFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>          </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>CÔNG TY</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>CỔ PHẦN ĐẦU T</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="vi-VN" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Ư</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> LIÊN DOANH VIỆT ANH</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>          </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Cụm  Cụm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Công nghiệp Liên Ph</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="vi-VN" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>ươn</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>g-Th</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="vi-VN" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>ườ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1100" b="1">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>ng Tín-Hà Nội</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="4" name="Picture 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{676B4BF4-916F-4710-A652-86DF7BC53E22}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2496,7 +2792,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D11DA811-16F8-4498-A727-A24BACB927DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D11DA811-16F8-4498-A727-A24BACB927DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2804,55 +3100,55 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X4" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="X4" workbookViewId="0">
       <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1796875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="5" width="13.81640625" style="1" customWidth="1"/>
-    <col min="6" max="9" width="16.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="9" width="16.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="21" style="1" customWidth="1"/>
-    <col min="12" max="14" width="19.54296875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1796875" style="1" customWidth="1"/>
+    <col min="12" max="14" width="19.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="17" style="1" customWidth="1"/>
     <col min="17" max="17" width="16" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16.81640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="18.7265625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="17.54296875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="18.81640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" style="1" customWidth="1"/>
     <col min="22" max="24" width="14" style="1" customWidth="1"/>
     <col min="25" max="25" width="14" style="6" customWidth="1"/>
     <col min="26" max="29" width="14" style="1" customWidth="1"/>
-    <col min="30" max="30" width="16.26953125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="17.1796875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="14.7265625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="17.7265625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="16.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="17.140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" style="1" customWidth="1"/>
+    <col min="33" max="33" width="17.7109375" style="1" customWidth="1"/>
     <col min="34" max="34" width="22" style="1" customWidth="1"/>
-    <col min="35" max="35" width="18.54296875" style="1" customWidth="1"/>
-    <col min="36" max="36" width="22.26953125" style="1" customWidth="1"/>
-    <col min="37" max="37" width="23.26953125" style="1" customWidth="1"/>
-    <col min="38" max="38" width="19.54296875" style="1" customWidth="1"/>
+    <col min="35" max="35" width="18.5703125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="22.28515625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="23.28515625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="19.5703125" style="1" customWidth="1"/>
     <col min="39" max="45" width="14" style="1" customWidth="1"/>
     <col min="46" max="46" width="14" style="7" customWidth="1"/>
-    <col min="47" max="16384" width="9.1796875" style="7"/>
+    <col min="47" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -2898,7 +3194,7 @@
       <c r="AR1" s="7"/>
       <c r="AS1" s="7"/>
     </row>
-    <row r="2" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2944,7 +3240,7 @@
       <c r="AR2" s="7"/>
       <c r="AS2" s="7"/>
     </row>
-    <row r="3" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -2990,7 +3286,7 @@
       <c r="AR3" s="7"/>
       <c r="AS3" s="7"/>
     </row>
-    <row r="4" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -3036,7 +3332,7 @@
       <c r="AR4" s="7"/>
       <c r="AS4" s="7"/>
     </row>
-    <row r="5" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -3082,7 +3378,7 @@
       <c r="AR5" s="7"/>
       <c r="AS5" s="7"/>
     </row>
-    <row r="6" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -3128,7 +3424,7 @@
       <c r="AR6" s="7"/>
       <c r="AS6" s="7"/>
     </row>
-    <row r="7" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -3174,7 +3470,7 @@
       <c r="AR7" s="7"/>
       <c r="AS7" s="7"/>
     </row>
-    <row r="8" spans="1:48" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:48" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -3315,7 +3611,7 @@
       </c>
       <c r="AV8" s="13"/>
     </row>
-    <row r="9" spans="1:48" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:48" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -3455,7 +3751,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:48" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>81</v>
       </c>
@@ -3595,7 +3891,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3643,7 +3939,7 @@
       <c r="AS11" s="2"/>
       <c r="AT11" s="2"/>
     </row>
-    <row r="12" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:48" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3691,7 +3987,7 @@
       <c r="AS12" s="2"/>
       <c r="AT12" s="2"/>
     </row>
-    <row r="13" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3739,19 +4035,19 @@
       <c r="AS13" s="2"/>
       <c r="AT13" s="2"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="AA14" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q9" r:id="rId1"/>
-    <hyperlink ref="AL9" r:id="rId2"/>
-    <hyperlink ref="AD9" r:id="rId3"/>
-    <hyperlink ref="AE9" r:id="rId4"/>
-    <hyperlink ref="Q10" r:id="rId5"/>
-    <hyperlink ref="AL10" r:id="rId6"/>
-    <hyperlink ref="AD10" r:id="rId7"/>
-    <hyperlink ref="AE10" r:id="rId8"/>
+    <hyperlink ref="Q9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="AL9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="AD9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="AE9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="Q10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="AL10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="AD10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="AE10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
@@ -3759,19 +4055,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Cấu hình - Drop down list'!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>N9:N13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Cấu hình - Drop down list'!$B$2:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>Y9:Y13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Cấu hình - Drop down list'!$C$2:$C$7</xm:f>
           </x14:formula1>
@@ -3784,21 +4080,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" style="7" customWidth="1"/>
-    <col min="2" max="7" width="19.54296875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="7"/>
+    <col min="1" max="1" width="19.5703125" style="7" customWidth="1"/>
+    <col min="2" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -3806,7 +4102,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3814,7 +4110,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -3822,7 +4118,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -3830,7 +4126,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -3839,7 +4135,7 @@
       <c r="G5" s="7"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -3847,7 +4143,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -3855,7 +4151,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -3879,7 +4175,7 @@
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -3902,7 +4198,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>81</v>
       </c>
@@ -3960,71 +4256,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="7" customWidth="1"/>
     <col min="2" max="6" width="20" style="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="7"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -4048,7 +4344,7 @@
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -4071,7 +4367,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>81</v>
       </c>
@@ -4094,7 +4390,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>117</v>
       </c>
@@ -4117,7 +4413,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>133</v>
       </c>
@@ -4140,7 +4436,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>134</v>
       </c>
@@ -4170,7 +4466,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>'Cấu hình - Drop down list'!$D$2:$D$6</xm:f>
           </x14:formula1>
@@ -4183,71 +4479,71 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" style="7" customWidth="1"/>
-    <col min="2" max="6" width="19.81640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="7"/>
+    <col min="1" max="1" width="19.85546875" style="7" customWidth="1"/>
+    <col min="2" max="6" width="19.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -4271,7 +4567,7 @@
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -4294,7 +4590,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>81</v>
       </c>
@@ -4352,71 +4648,71 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" style="7" customWidth="1"/>
-    <col min="2" max="6" width="20.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="7"/>
+    <col min="1" max="1" width="20.42578125" style="7" customWidth="1"/>
+    <col min="2" max="6" width="20.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -4440,7 +4736,7 @@
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -4463,7 +4759,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>81</v>
       </c>
@@ -4522,71 +4818,78 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D43B45E-1A5D-4D90-BCA0-87A04D697F3F}">
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="7" customWidth="1"/>
-    <col min="2" max="6" width="23" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="7"/>
+    <col min="1" max="1" width="19.5703125" style="7" customWidth="1"/>
+    <col min="2" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="G5" s="7"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -4597,6 +4900,175 @@
         <v>2</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" style="7" customWidth="1"/>
+    <col min="2" max="6" width="23" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>122</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -4610,7 +5082,7 @@
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -4633,7 +5105,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>81</v>
       </c>
@@ -4656,7 +5128,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>117</v>
       </c>
@@ -4704,7 +5176,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>'Cấu hình - Drop down list'!$E$2:$E$4</xm:f>
           </x14:formula1>
@@ -4716,23 +5188,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -4749,7 +5221,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>53</v>
       </c>
@@ -4766,7 +5238,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>144</v>
       </c>
@@ -4783,7 +5255,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>146</v>
       </c>
@@ -4797,7 +5269,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>147</v>
       </c>
@@ -4808,7 +5280,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="18" t="s">
         <v>150</v>
       </c>
@@ -4816,7 +5288,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="18" t="s">
         <v>152</v>
       </c>

</xml_diff>